<commit_message>
Decho's version of the plan
</commit_message>
<xml_diff>
--- a/TestPlan/Distribution of Teamwork.xlsx
+++ b/TestPlan/Distribution of Teamwork.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Decho\Desktop\TeamLich\Week 3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Decho\Desktop\TestsAndPlans\TestPlan\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -495,7 +495,7 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added sample test case management Excel spreadsheet, and added a function difficulty spreadsheet
</commit_message>
<xml_diff>
--- a/TestPlan/Distribution of Teamwork.xlsx
+++ b/TestPlan/Distribution of Teamwork.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="39">
   <si>
     <t>Настройки</t>
   </si>
@@ -139,13 +139,22 @@
   </si>
   <si>
     <t>Календар</t>
+  </si>
+  <si>
+    <t>Medium</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>Low</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -153,8 +162,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -164,6 +179,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -180,10 +213,30 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Нормален" xfId="0" builtinId="0"/>
@@ -492,78 +545,88 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="83.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.42578125" style="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="7" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="D1" s="9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="B2" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="B3" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="B4" s="10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="B5" s="9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="B6" s="9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="B7" s="8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="8" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>